<commit_message>
Módulo 09 - Projeto estoque part 02
</commit_message>
<xml_diff>
--- a/projeto estoque/Projeto estoque.xlsx
+++ b/projeto estoque/Projeto estoque.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="8670" windowHeight="6180" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="8670" windowHeight="6180"/>
   </bookViews>
   <sheets>
     <sheet name="Início" sheetId="1" r:id="rId1"/>
@@ -324,6 +324,430 @@
             </a:rPr>
             <a:t>Lançamentos</a:t>
           </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>33337</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>104775</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>576262</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>41911</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="5" name="CaixaDeTexto 4"/>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="4843462" y="1495425"/>
+          <a:ext cx="2638425" cy="889636"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="lt1"/>
+        </a:solidFill>
+        <a:ln w="9525" cmpd="sng">
+          <a:noFill/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="ctr"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr lang="pt-BR" sz="2000" b="1"/>
+            <a:t>Controle de estoques </a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr lang="pt-BR" sz="2000" b="1"/>
+            <a:t>Simplificado</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>933449</xdr:colOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>85725</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>723900</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>47625</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="6" name="CaixaDeTexto 5"/>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="3648074" y="2809875"/>
+          <a:ext cx="5029201" cy="1295400"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="lt1"/>
+        </a:solidFill>
+        <a:ln w="9525" cmpd="sng">
+          <a:noFill/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr lang="pt-BR" sz="1200" b="1"/>
+            <a:t>Orientações</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:endParaRPr lang="pt-BR" sz="1200" b="1"/>
+        </a:p>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr lang="pt-BR" sz="1200"/>
+            <a:t>1. Cadastrar o produto na aba "Cadastro".</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr lang="pt-BR" sz="1200"/>
+            <a:t>2. Registrar as entradas e saídas na aba "Lançamentos".</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr lang="pt-BR" sz="1200"/>
+            <a:t>3. Relatórios e consultas usar os filtros nas abas "Cadastro" e "Lançamentos".</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>2108950</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="2226635" cy="655949"/>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="7" name="CaixaDeTexto 6"/>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="10062325" y="0"/>
+          <a:ext cx="2226635" cy="655949"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="none" rtlCol="0" anchor="t">
+          <a:spAutoFit/>
+        </a:bodyPr>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr lang="pt-BR" sz="1800" b="1" cap="none" spc="0">
+              <a:ln w="0"/>
+              <a:gradFill>
+                <a:gsLst>
+                  <a:gs pos="0">
+                    <a:schemeClr val="accent5">
+                      <a:lumMod val="50000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                  <a:gs pos="50000">
+                    <a:schemeClr val="accent5"/>
+                  </a:gs>
+                  <a:gs pos="100000">
+                    <a:schemeClr val="accent5">
+                      <a:lumMod val="60000"/>
+                      <a:lumOff val="40000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                </a:gsLst>
+                <a:lin ang="5400000"/>
+              </a:gradFill>
+              <a:effectLst>
+                <a:reflection blurRad="6350" stA="53000" endA="300" endPos="35500" dir="5400000" sy="-90000" algn="bl" rotWithShape="0"/>
+              </a:effectLst>
+            </a:rPr>
+            <a:t>JS </a:t>
+          </a:r>
+          <a:endParaRPr lang="pt-BR" sz="1800" b="1" cap="none" spc="0" baseline="0">
+            <a:ln w="0"/>
+            <a:gradFill>
+              <a:gsLst>
+                <a:gs pos="0">
+                  <a:schemeClr val="accent5">
+                    <a:lumMod val="50000"/>
+                  </a:schemeClr>
+                </a:gs>
+                <a:gs pos="50000">
+                  <a:schemeClr val="accent5"/>
+                </a:gs>
+                <a:gs pos="100000">
+                  <a:schemeClr val="accent5">
+                    <a:lumMod val="60000"/>
+                    <a:lumOff val="40000"/>
+                  </a:schemeClr>
+                </a:gs>
+              </a:gsLst>
+              <a:lin ang="5400000"/>
+            </a:gradFill>
+            <a:effectLst>
+              <a:reflection blurRad="6350" stA="53000" endA="300" endPos="35500" dir="5400000" sy="-90000" algn="bl" rotWithShape="0"/>
+            </a:effectLst>
+          </a:endParaRPr>
+        </a:p>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr lang="pt-BR" sz="1800" b="1" cap="none" spc="0">
+              <a:ln w="0"/>
+              <a:gradFill>
+                <a:gsLst>
+                  <a:gs pos="0">
+                    <a:schemeClr val="accent5">
+                      <a:lumMod val="50000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                  <a:gs pos="50000">
+                    <a:schemeClr val="accent5"/>
+                  </a:gs>
+                  <a:gs pos="100000">
+                    <a:schemeClr val="accent5">
+                      <a:lumMod val="60000"/>
+                      <a:lumOff val="40000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                </a:gsLst>
+                <a:lin ang="5400000"/>
+              </a:gradFill>
+              <a:effectLst>
+                <a:reflection blurRad="6350" stA="53000" endA="300" endPos="35500" dir="5400000" sy="-90000" algn="bl" rotWithShape="0"/>
+              </a:effectLst>
+            </a:rPr>
+            <a:t>Controle</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="pt-BR" sz="1800" b="1" cap="none" spc="0" baseline="0">
+              <a:ln w="0"/>
+              <a:gradFill>
+                <a:gsLst>
+                  <a:gs pos="0">
+                    <a:schemeClr val="accent5">
+                      <a:lumMod val="50000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                  <a:gs pos="50000">
+                    <a:schemeClr val="accent5"/>
+                  </a:gs>
+                  <a:gs pos="100000">
+                    <a:schemeClr val="accent5">
+                      <a:lumMod val="60000"/>
+                      <a:lumOff val="40000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                </a:gsLst>
+                <a:lin ang="5400000"/>
+              </a:gradFill>
+              <a:effectLst>
+                <a:reflection blurRad="6350" stA="53000" endA="300" endPos="35500" dir="5400000" sy="-90000" algn="bl" rotWithShape="0"/>
+              </a:effectLst>
+            </a:rPr>
+            <a:t> de estoques</a:t>
+          </a:r>
+          <a:endParaRPr lang="pt-BR" sz="1800" b="1" cap="none" spc="0">
+            <a:ln w="0"/>
+            <a:gradFill>
+              <a:gsLst>
+                <a:gs pos="0">
+                  <a:schemeClr val="accent5">
+                    <a:lumMod val="50000"/>
+                  </a:schemeClr>
+                </a:gs>
+                <a:gs pos="50000">
+                  <a:schemeClr val="accent5"/>
+                </a:gs>
+                <a:gs pos="100000">
+                  <a:schemeClr val="accent5">
+                    <a:lumMod val="60000"/>
+                    <a:lumOff val="40000"/>
+                  </a:schemeClr>
+                </a:gs>
+              </a:gsLst>
+              <a:lin ang="5400000"/>
+            </a:gradFill>
+            <a:effectLst>
+              <a:reflection blurRad="6350" stA="53000" endA="300" endPos="35500" dir="5400000" sy="-90000" algn="bl" rotWithShape="0"/>
+            </a:effectLst>
+          </a:endParaRPr>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>3448051</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>85725</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>3686175</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>314325</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="8" name="Estrela de 4 pontas 7"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="11401426" y="85725"/>
+          <a:ext cx="238124" cy="228600"/>
+        </a:xfrm>
+        <a:prstGeom prst="star4">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="accent6"/>
+        </a:solidFill>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="pt-BR" sz="1100" b="0" cap="none" spc="0">
+            <a:ln w="0"/>
+            <a:gradFill>
+              <a:gsLst>
+                <a:gs pos="0">
+                  <a:schemeClr val="accent5">
+                    <a:lumMod val="50000"/>
+                  </a:schemeClr>
+                </a:gs>
+                <a:gs pos="50000">
+                  <a:schemeClr val="accent5"/>
+                </a:gs>
+                <a:gs pos="100000">
+                  <a:schemeClr val="accent5">
+                    <a:lumMod val="60000"/>
+                    <a:lumOff val="40000"/>
+                  </a:schemeClr>
+                </a:gs>
+              </a:gsLst>
+              <a:lin ang="5400000"/>
+            </a:gradFill>
+            <a:effectLst>
+              <a:reflection blurRad="6350" stA="53000" endA="300" endPos="35500" dir="5400000" sy="-90000" algn="bl" rotWithShape="0"/>
+            </a:effectLst>
+          </a:endParaRPr>
         </a:p>
       </xdr:txBody>
     </xdr:sp>
@@ -1047,7 +1471,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G1"/>
   <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0"/>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+      <selection activeCell="G16" sqref="G16"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="0" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -1057,7 +1483,7 @@
     <col min="8" max="16384" width="9.140625" hidden="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -1069,6 +1495,7 @@
       <c r="G1" s="1"/>
     </row>
   </sheetData>
+  <sheetProtection algorithmName="SHA-512" hashValue="/2DTNwpdLfDoZzJJ/JrD8Siw7Q4pJTMke8+Cmq5X6gzihE+tx3WF3edUvstUj5HKhGwv6frgLvfppzOzdZUEfw==" saltValue="Fj+ngRhWi2/1Z9nx6oB1qw==" spinCount="100000" sheet="1" objects="1" scenarios="1" selectLockedCells="1"/>
   <hyperlinks>
     <hyperlink ref="A1" location="Início!G1" display="Início!G1"/>
   </hyperlinks>
@@ -1119,7 +1546,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G1"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+    <sheetView showGridLines="0" workbookViewId="0">
       <selection activeCell="G1" sqref="G1"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Módulo 09 - Projeto estoque part 03
</commit_message>
<xml_diff>
--- a/projeto estoque/Projeto estoque.xlsx
+++ b/projeto estoque/Projeto estoque.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="8670" windowHeight="6180"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="8670" windowHeight="6180" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Início" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="16">
   <si>
     <t>Início!G1</t>
   </si>
@@ -36,12 +36,53 @@
   <si>
     <t>Cadastro!G1</t>
   </si>
+  <si>
+    <t>Produto</t>
+  </si>
+  <si>
+    <t>Medida</t>
+  </si>
+  <si>
+    <t>Estoque
+mínimo</t>
+  </si>
+  <si>
+    <t>Estoque
+máximo</t>
+  </si>
+  <si>
+    <t>Saldo</t>
+  </si>
+  <si>
+    <t>Avisos</t>
+  </si>
+  <si>
+    <t>Caneta esferográfica azul</t>
+  </si>
+  <si>
+    <t>Caneta esferográfica preta</t>
+  </si>
+  <si>
+    <t>Unidade</t>
+  </si>
+  <si>
+    <t>Data</t>
+  </si>
+  <si>
+    <t>Saída</t>
+  </si>
+  <si>
+    <t>Entrada</t>
+  </si>
+  <si>
+    <t>Total</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -57,8 +98,39 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color rgb="FFC00000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="9" tint="-0.249977111117893"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="13"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -68,6 +140,18 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="0" tint="-4.9989318521683403E-2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.249977111117893"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.14999847407452621"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -85,16 +169,151 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="14" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hiperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="14">
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="0" tint="-0.14999847407452621"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="0" tint="-0.14999847407452621"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="13"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="19" formatCode="dd/mm/yyyy"/>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="0" tint="-0.249977111117893"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="13"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="1" formatCode="0"/>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="0" tint="-0.14999847407452621"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="1" formatCode="0"/>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="0" tint="-0.249977111117893"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="1" formatCode="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="1" formatCode="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="19" formatCode="dd/mm/yyyy"/>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="0" tint="-0.14999847407452621"/>
+        </patternFill>
+      </fill>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -978,6 +1197,276 @@
     </xdr:sp>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>2107240</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="2226635" cy="655949"/>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="5" name="CaixaDeTexto 4"/>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="10060615" y="0"/>
+          <a:ext cx="2226635" cy="655949"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="none" rtlCol="0" anchor="t">
+          <a:spAutoFit/>
+        </a:bodyPr>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr lang="pt-BR" sz="1800" b="1" cap="none" spc="0">
+              <a:ln w="0"/>
+              <a:gradFill>
+                <a:gsLst>
+                  <a:gs pos="0">
+                    <a:schemeClr val="accent5">
+                      <a:lumMod val="50000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                  <a:gs pos="50000">
+                    <a:schemeClr val="accent5"/>
+                  </a:gs>
+                  <a:gs pos="100000">
+                    <a:schemeClr val="accent5">
+                      <a:lumMod val="60000"/>
+                      <a:lumOff val="40000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                </a:gsLst>
+                <a:lin ang="5400000"/>
+              </a:gradFill>
+              <a:effectLst>
+                <a:reflection blurRad="6350" stA="53000" endA="300" endPos="35500" dir="5400000" sy="-90000" algn="bl" rotWithShape="0"/>
+              </a:effectLst>
+            </a:rPr>
+            <a:t>JS </a:t>
+          </a:r>
+          <a:endParaRPr lang="pt-BR" sz="1800" b="1" cap="none" spc="0" baseline="0">
+            <a:ln w="0"/>
+            <a:gradFill>
+              <a:gsLst>
+                <a:gs pos="0">
+                  <a:schemeClr val="accent5">
+                    <a:lumMod val="50000"/>
+                  </a:schemeClr>
+                </a:gs>
+                <a:gs pos="50000">
+                  <a:schemeClr val="accent5"/>
+                </a:gs>
+                <a:gs pos="100000">
+                  <a:schemeClr val="accent5">
+                    <a:lumMod val="60000"/>
+                    <a:lumOff val="40000"/>
+                  </a:schemeClr>
+                </a:gs>
+              </a:gsLst>
+              <a:lin ang="5400000"/>
+            </a:gradFill>
+            <a:effectLst>
+              <a:reflection blurRad="6350" stA="53000" endA="300" endPos="35500" dir="5400000" sy="-90000" algn="bl" rotWithShape="0"/>
+            </a:effectLst>
+          </a:endParaRPr>
+        </a:p>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr lang="pt-BR" sz="1800" b="1" cap="none" spc="0">
+              <a:ln w="0"/>
+              <a:gradFill>
+                <a:gsLst>
+                  <a:gs pos="0">
+                    <a:schemeClr val="accent5">
+                      <a:lumMod val="50000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                  <a:gs pos="50000">
+                    <a:schemeClr val="accent5"/>
+                  </a:gs>
+                  <a:gs pos="100000">
+                    <a:schemeClr val="accent5">
+                      <a:lumMod val="60000"/>
+                      <a:lumOff val="40000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                </a:gsLst>
+                <a:lin ang="5400000"/>
+              </a:gradFill>
+              <a:effectLst>
+                <a:reflection blurRad="6350" stA="53000" endA="300" endPos="35500" dir="5400000" sy="-90000" algn="bl" rotWithShape="0"/>
+              </a:effectLst>
+            </a:rPr>
+            <a:t>Controle</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="pt-BR" sz="1800" b="1" cap="none" spc="0" baseline="0">
+              <a:ln w="0"/>
+              <a:gradFill>
+                <a:gsLst>
+                  <a:gs pos="0">
+                    <a:schemeClr val="accent5">
+                      <a:lumMod val="50000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                  <a:gs pos="50000">
+                    <a:schemeClr val="accent5"/>
+                  </a:gs>
+                  <a:gs pos="100000">
+                    <a:schemeClr val="accent5">
+                      <a:lumMod val="60000"/>
+                      <a:lumOff val="40000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                </a:gsLst>
+                <a:lin ang="5400000"/>
+              </a:gradFill>
+              <a:effectLst>
+                <a:reflection blurRad="6350" stA="53000" endA="300" endPos="35500" dir="5400000" sy="-90000" algn="bl" rotWithShape="0"/>
+              </a:effectLst>
+            </a:rPr>
+            <a:t> de estoques</a:t>
+          </a:r>
+          <a:endParaRPr lang="pt-BR" sz="1800" b="1" cap="none" spc="0">
+            <a:ln w="0"/>
+            <a:gradFill>
+              <a:gsLst>
+                <a:gs pos="0">
+                  <a:schemeClr val="accent5">
+                    <a:lumMod val="50000"/>
+                  </a:schemeClr>
+                </a:gs>
+                <a:gs pos="50000">
+                  <a:schemeClr val="accent5"/>
+                </a:gs>
+                <a:gs pos="100000">
+                  <a:schemeClr val="accent5">
+                    <a:lumMod val="60000"/>
+                    <a:lumOff val="40000"/>
+                  </a:schemeClr>
+                </a:gs>
+              </a:gsLst>
+              <a:lin ang="5400000"/>
+            </a:gradFill>
+            <a:effectLst>
+              <a:reflection blurRad="6350" stA="53000" endA="300" endPos="35500" dir="5400000" sy="-90000" algn="bl" rotWithShape="0"/>
+            </a:effectLst>
+          </a:endParaRPr>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>3450265</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>85725</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>3688389</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>314325</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="6" name="Estrela de 4 pontas 5"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="11403640" y="85725"/>
+          <a:ext cx="238124" cy="228600"/>
+        </a:xfrm>
+        <a:prstGeom prst="star4">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="accent6"/>
+        </a:solidFill>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="pt-BR" sz="1100" b="0" cap="none" spc="0">
+            <a:ln w="0"/>
+            <a:gradFill>
+              <a:gsLst>
+                <a:gs pos="0">
+                  <a:schemeClr val="accent5">
+                    <a:lumMod val="50000"/>
+                  </a:schemeClr>
+                </a:gs>
+                <a:gs pos="50000">
+                  <a:schemeClr val="accent5"/>
+                </a:gs>
+                <a:gs pos="100000">
+                  <a:schemeClr val="accent5">
+                    <a:lumMod val="60000"/>
+                    <a:lumOff val="40000"/>
+                  </a:schemeClr>
+                </a:gs>
+              </a:gsLst>
+              <a:lin ang="5400000"/>
+            </a:gradFill>
+            <a:effectLst>
+              <a:reflection blurRad="6350" stA="53000" endA="300" endPos="35500" dir="5400000" sy="-90000" algn="bl" rotWithShape="0"/>
+            </a:effectLst>
+          </a:endParaRPr>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
 
@@ -1203,7 +1692,306 @@
     </xdr:sp>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>2105025</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="2226635" cy="655949"/>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="5" name="CaixaDeTexto 4"/>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="10058400" y="0"/>
+          <a:ext cx="2226635" cy="655949"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="none" rtlCol="0" anchor="t">
+          <a:spAutoFit/>
+        </a:bodyPr>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr lang="pt-BR" sz="1800" b="1" cap="none" spc="0">
+              <a:ln w="0"/>
+              <a:gradFill>
+                <a:gsLst>
+                  <a:gs pos="0">
+                    <a:schemeClr val="accent5">
+                      <a:lumMod val="50000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                  <a:gs pos="50000">
+                    <a:schemeClr val="accent5"/>
+                  </a:gs>
+                  <a:gs pos="100000">
+                    <a:schemeClr val="accent5">
+                      <a:lumMod val="60000"/>
+                      <a:lumOff val="40000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                </a:gsLst>
+                <a:lin ang="5400000"/>
+              </a:gradFill>
+              <a:effectLst>
+                <a:reflection blurRad="6350" stA="53000" endA="300" endPos="35500" dir="5400000" sy="-90000" algn="bl" rotWithShape="0"/>
+              </a:effectLst>
+            </a:rPr>
+            <a:t>JS </a:t>
+          </a:r>
+          <a:endParaRPr lang="pt-BR" sz="1800" b="1" cap="none" spc="0" baseline="0">
+            <a:ln w="0"/>
+            <a:gradFill>
+              <a:gsLst>
+                <a:gs pos="0">
+                  <a:schemeClr val="accent5">
+                    <a:lumMod val="50000"/>
+                  </a:schemeClr>
+                </a:gs>
+                <a:gs pos="50000">
+                  <a:schemeClr val="accent5"/>
+                </a:gs>
+                <a:gs pos="100000">
+                  <a:schemeClr val="accent5">
+                    <a:lumMod val="60000"/>
+                    <a:lumOff val="40000"/>
+                  </a:schemeClr>
+                </a:gs>
+              </a:gsLst>
+              <a:lin ang="5400000"/>
+            </a:gradFill>
+            <a:effectLst>
+              <a:reflection blurRad="6350" stA="53000" endA="300" endPos="35500" dir="5400000" sy="-90000" algn="bl" rotWithShape="0"/>
+            </a:effectLst>
+          </a:endParaRPr>
+        </a:p>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr lang="pt-BR" sz="1800" b="1" cap="none" spc="0">
+              <a:ln w="0"/>
+              <a:gradFill>
+                <a:gsLst>
+                  <a:gs pos="0">
+                    <a:schemeClr val="accent5">
+                      <a:lumMod val="50000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                  <a:gs pos="50000">
+                    <a:schemeClr val="accent5"/>
+                  </a:gs>
+                  <a:gs pos="100000">
+                    <a:schemeClr val="accent5">
+                      <a:lumMod val="60000"/>
+                      <a:lumOff val="40000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                </a:gsLst>
+                <a:lin ang="5400000"/>
+              </a:gradFill>
+              <a:effectLst>
+                <a:reflection blurRad="6350" stA="53000" endA="300" endPos="35500" dir="5400000" sy="-90000" algn="bl" rotWithShape="0"/>
+              </a:effectLst>
+            </a:rPr>
+            <a:t>Controle</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="pt-BR" sz="1800" b="1" cap="none" spc="0" baseline="0">
+              <a:ln w="0"/>
+              <a:gradFill>
+                <a:gsLst>
+                  <a:gs pos="0">
+                    <a:schemeClr val="accent5">
+                      <a:lumMod val="50000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                  <a:gs pos="50000">
+                    <a:schemeClr val="accent5"/>
+                  </a:gs>
+                  <a:gs pos="100000">
+                    <a:schemeClr val="accent5">
+                      <a:lumMod val="60000"/>
+                      <a:lumOff val="40000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                </a:gsLst>
+                <a:lin ang="5400000"/>
+              </a:gradFill>
+              <a:effectLst>
+                <a:reflection blurRad="6350" stA="53000" endA="300" endPos="35500" dir="5400000" sy="-90000" algn="bl" rotWithShape="0"/>
+              </a:effectLst>
+            </a:rPr>
+            <a:t> de estoques</a:t>
+          </a:r>
+          <a:endParaRPr lang="pt-BR" sz="1800" b="1" cap="none" spc="0">
+            <a:ln w="0"/>
+            <a:gradFill>
+              <a:gsLst>
+                <a:gs pos="0">
+                  <a:schemeClr val="accent5">
+                    <a:lumMod val="50000"/>
+                  </a:schemeClr>
+                </a:gs>
+                <a:gs pos="50000">
+                  <a:schemeClr val="accent5"/>
+                </a:gs>
+                <a:gs pos="100000">
+                  <a:schemeClr val="accent5">
+                    <a:lumMod val="60000"/>
+                    <a:lumOff val="40000"/>
+                  </a:schemeClr>
+                </a:gs>
+              </a:gsLst>
+              <a:lin ang="5400000"/>
+            </a:gradFill>
+            <a:effectLst>
+              <a:reflection blurRad="6350" stA="53000" endA="300" endPos="35500" dir="5400000" sy="-90000" algn="bl" rotWithShape="0"/>
+            </a:effectLst>
+          </a:endParaRPr>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>3448050</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>85725</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>3686174</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>314325</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="6" name="Estrela de 4 pontas 5"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="11401425" y="85725"/>
+          <a:ext cx="238124" cy="228600"/>
+        </a:xfrm>
+        <a:prstGeom prst="star4">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="accent6"/>
+        </a:solidFill>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="pt-BR" sz="1100" b="0" cap="none" spc="0">
+            <a:ln w="0"/>
+            <a:gradFill>
+              <a:gsLst>
+                <a:gs pos="0">
+                  <a:schemeClr val="accent5">
+                    <a:lumMod val="50000"/>
+                  </a:schemeClr>
+                </a:gs>
+                <a:gs pos="50000">
+                  <a:schemeClr val="accent5"/>
+                </a:gs>
+                <a:gs pos="100000">
+                  <a:schemeClr val="accent5">
+                    <a:lumMod val="60000"/>
+                    <a:lumOff val="40000"/>
+                  </a:schemeClr>
+                </a:gs>
+              </a:gsLst>
+              <a:lin ang="5400000"/>
+            </a:gradFill>
+            <a:effectLst>
+              <a:reflection blurRad="6350" stA="53000" endA="300" endPos="35500" dir="5400000" sy="-90000" algn="bl" rotWithShape="0"/>
+            </a:effectLst>
+          </a:endParaRPr>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
 </xdr:wsDr>
+</file>
+
+<file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="TbCadastro" displayName="TbCadastro" ref="A3:F8" totalsRowCount="1" headerRowDxfId="5">
+  <autoFilter ref="A3:F7"/>
+  <tableColumns count="6">
+    <tableColumn id="1" name="Produto" totalsRowLabel="Total"/>
+    <tableColumn id="2" name="Medida"/>
+    <tableColumn id="3" name="Estoque_x000a_mínimo" dataDxfId="8"/>
+    <tableColumn id="4" name="Estoque_x000a_máximo" dataDxfId="6"/>
+    <tableColumn id="5" name="Saldo" dataDxfId="7" totalsRowDxfId="1"/>
+    <tableColumn id="6" name="Avisos" totalsRowFunction="count" dataDxfId="13" totalsRowDxfId="0"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium25" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="TbLancamentos" displayName="TbLancamentos" ref="A3:E8" totalsRowCount="1" headerRowDxfId="2">
+  <autoFilter ref="A3:E7"/>
+  <tableColumns count="5">
+    <tableColumn id="1" name="Produto" totalsRowLabel="Total"/>
+    <tableColumn id="2" name="Data" totalsRowFunction="count" dataDxfId="12" totalsRowDxfId="3"/>
+    <tableColumn id="3" name="Entrada" totalsRowFunction="sum" dataDxfId="11"/>
+    <tableColumn id="4" name="Saída" totalsRowFunction="sum" dataDxfId="10"/>
+    <tableColumn id="5" name="Saldo" totalsRowFunction="count" dataDxfId="9" totalsRowDxfId="4"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium25" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1471,8 +2259,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G1"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="G16" sqref="G16"/>
+    <sheetView showGridLines="0" workbookViewId="0">
+      <selection activeCell="A14" sqref="A14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="0" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1495,7 +2283,7 @@
       <c r="G1" s="1"/>
     </row>
   </sheetData>
-  <sheetProtection algorithmName="SHA-512" hashValue="/2DTNwpdLfDoZzJJ/JrD8Siw7Q4pJTMke8+Cmq5X6gzihE+tx3WF3edUvstUj5HKhGwv6frgLvfppzOzdZUEfw==" saltValue="Fj+ngRhWi2/1Z9nx6oB1qw==" spinCount="100000" sheet="1" objects="1" scenarios="1" selectLockedCells="1"/>
+  <sheetProtection sheet="1" objects="1" scenarios="1" selectLockedCells="1"/>
   <hyperlinks>
     <hyperlink ref="A1" location="Início!G1" display="Início!G1"/>
   </hyperlinks>
@@ -1507,10 +2295,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G1"/>
+  <dimension ref="A1:G8"/>
   <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="G1" sqref="G1"/>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+      <selection activeCell="G3" sqref="G3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="0" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1521,7 +2309,7 @@
     <col min="8" max="16384" width="9.140625" hidden="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>2</v>
       </c>
@@ -1531,6 +2319,80 @@
       <c r="E1" s="1"/>
       <c r="F1" s="1"/>
       <c r="G1" s="1"/>
+    </row>
+    <row r="3" spans="1:7" s="3" customFormat="1" ht="34.5" x14ac:dyDescent="0.25">
+      <c r="A3" s="14" t="s">
+        <v>3</v>
+      </c>
+      <c r="B3" s="9" t="s">
+        <v>4</v>
+      </c>
+      <c r="C3" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="D3" s="10" t="s">
+        <v>6</v>
+      </c>
+      <c r="E3" s="11" t="s">
+        <v>7</v>
+      </c>
+      <c r="F3" s="11" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>9</v>
+      </c>
+      <c r="B4" t="s">
+        <v>11</v>
+      </c>
+      <c r="C4" s="12">
+        <v>15</v>
+      </c>
+      <c r="D4" s="12">
+        <v>150</v>
+      </c>
+      <c r="E4" s="5"/>
+      <c r="F4" s="5"/>
+    </row>
+    <row r="5" spans="1:7" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>10</v>
+      </c>
+      <c r="B5" t="s">
+        <v>11</v>
+      </c>
+      <c r="C5" s="12">
+        <v>15</v>
+      </c>
+      <c r="D5" s="12">
+        <v>150</v>
+      </c>
+      <c r="E5" s="5"/>
+      <c r="F5" s="5"/>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="C6" s="12"/>
+      <c r="D6" s="12"/>
+      <c r="E6" s="5"/>
+      <c r="F6" s="5"/>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="C7" s="12"/>
+      <c r="D7" s="12"/>
+      <c r="E7" s="5"/>
+      <c r="F7" s="5"/>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>15</v>
+      </c>
+      <c r="E8" s="5"/>
+      <c r="F8" s="5">
+        <f>SUBTOTAL(103,TbCadastro[Avisos])</f>
+        <v>0</v>
+      </c>
     </row>
   </sheetData>
   <hyperlinks>
@@ -1539,15 +2401,18 @@
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
   <drawing r:id="rId2"/>
+  <tableParts count="1">
+    <tablePart r:id="rId3"/>
+  </tableParts>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G1"/>
+  <dimension ref="A1:G8"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="G1" sqref="G1"/>
+      <selection activeCell="A7" sqref="A7:XFD7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="0" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1558,7 +2423,7 @@
     <col min="8" max="16384" width="9.140625" hidden="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>1</v>
       </c>
@@ -1568,6 +2433,86 @@
       <c r="E1" s="1"/>
       <c r="F1" s="1"/>
       <c r="G1" s="1"/>
+    </row>
+    <row r="3" spans="1:7" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="16" t="s">
+        <v>3</v>
+      </c>
+      <c r="B3" s="17" t="s">
+        <v>12</v>
+      </c>
+      <c r="C3" s="18" t="s">
+        <v>14</v>
+      </c>
+      <c r="D3" s="19" t="s">
+        <v>13</v>
+      </c>
+      <c r="E3" s="16" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>9</v>
+      </c>
+      <c r="B4" s="7">
+        <v>44978</v>
+      </c>
+      <c r="C4" s="12">
+        <v>20</v>
+      </c>
+      <c r="D4" s="12">
+        <v>10</v>
+      </c>
+      <c r="E4" s="13"/>
+    </row>
+    <row r="5" spans="1:7" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>10</v>
+      </c>
+      <c r="B5" s="8">
+        <v>44979</v>
+      </c>
+      <c r="C5" s="12">
+        <v>10</v>
+      </c>
+      <c r="D5" s="12">
+        <v>5</v>
+      </c>
+      <c r="E5" s="13"/>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B6" s="8"/>
+      <c r="C6" s="12"/>
+      <c r="D6" s="12"/>
+      <c r="E6" s="13"/>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B7" s="6"/>
+      <c r="C7" s="12"/>
+      <c r="D7" s="12"/>
+      <c r="E7" s="4"/>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>15</v>
+      </c>
+      <c r="B8" s="15">
+        <f>SUBTOTAL(103,TbLancamentos[Data])</f>
+        <v>2</v>
+      </c>
+      <c r="C8" s="12">
+        <f>SUBTOTAL(109,TbLancamentos[Entrada])</f>
+        <v>30</v>
+      </c>
+      <c r="D8" s="12">
+        <f>SUBTOTAL(109,TbLancamentos[Saída])</f>
+        <v>15</v>
+      </c>
+      <c r="E8" s="4">
+        <f>SUBTOTAL(103,TbLancamentos[Saldo])</f>
+        <v>0</v>
+      </c>
     </row>
   </sheetData>
   <hyperlinks>
@@ -1576,5 +2521,8 @@
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
   <drawing r:id="rId2"/>
+  <tableParts count="1">
+    <tablePart r:id="rId3"/>
+  </tableParts>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Módulo 09 - Projeto estoque part 04
</commit_message>
<xml_diff>
--- a/projeto estoque/Projeto estoque.xlsx
+++ b/projeto estoque/Projeto estoque.xlsx
@@ -9,13 +9,16 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="8670" windowHeight="6180" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="8670" windowHeight="6180" firstSheet="1" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Início" sheetId="1" r:id="rId1"/>
     <sheet name="Cadastro" sheetId="2" r:id="rId2"/>
     <sheet name="Lançamentos" sheetId="3" r:id="rId3"/>
   </sheets>
+  <definedNames>
+    <definedName name="ColunaProdutos">TbCadastro[Produto]</definedName>
+  </definedNames>
   <calcPr calcId="152511"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -26,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="16">
   <si>
     <t>Início!G1</t>
   </si>
@@ -75,7 +78,7 @@
     <t>Entrada</t>
   </si>
   <si>
-    <t>Total</t>
+    <t>Lápis</t>
   </si>
 </sst>
 </file>
@@ -169,7 +172,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1" applyFill="1"/>
@@ -178,7 +181,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
@@ -199,7 +201,6 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
@@ -217,7 +218,24 @@
     <cellStyle name="Hiperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="14">
+  <dxfs count="16">
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="1" formatCode="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="1" formatCode="0"/>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="0" tint="-0.249977111117893"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <fill>
         <patternFill patternType="solid">
@@ -233,60 +251,6 @@
           <bgColor theme="0" tint="-0.14999847407452621"/>
         </patternFill>
       </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="13"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <scheme val="minor"/>
-      </font>
-      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="19" formatCode="dd/mm/yyyy"/>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="0" tint="-0.249977111117893"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="13"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <scheme val="minor"/>
-      </font>
-      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="1" formatCode="0"/>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="0" tint="-0.14999847407452621"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="1" formatCode="0"/>
     </dxf>
     <dxf>
       <fill>
@@ -306,12 +270,55 @@
       <numFmt numFmtId="19" formatCode="dd/mm/yyyy"/>
     </dxf>
     <dxf>
+      <font>
+        <b/>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="13"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
       <fill>
         <patternFill patternType="solid">
           <fgColor indexed="64"/>
           <bgColor theme="0" tint="-0.14999847407452621"/>
         </patternFill>
       </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="0" tint="-0.14999847407452621"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="1" formatCode="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="1" formatCode="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="13"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -1966,29 +1973,29 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="TbCadastro" displayName="TbCadastro" ref="A3:F8" totalsRowCount="1" headerRowDxfId="5">
-  <autoFilter ref="A3:F7"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="TbCadastro" displayName="TbCadastro" ref="A3:F6" headerRowDxfId="15">
+  <autoFilter ref="A3:F6"/>
   <tableColumns count="6">
     <tableColumn id="1" name="Produto" totalsRowLabel="Total"/>
     <tableColumn id="2" name="Medida"/>
-    <tableColumn id="3" name="Estoque_x000a_mínimo" dataDxfId="8"/>
-    <tableColumn id="4" name="Estoque_x000a_máximo" dataDxfId="6"/>
-    <tableColumn id="5" name="Saldo" dataDxfId="7" totalsRowDxfId="1"/>
-    <tableColumn id="6" name="Avisos" totalsRowFunction="count" dataDxfId="13" totalsRowDxfId="0"/>
+    <tableColumn id="3" name="Estoque_x000a_mínimo" dataDxfId="14"/>
+    <tableColumn id="4" name="Estoque_x000a_máximo" dataDxfId="13"/>
+    <tableColumn id="5" name="Saldo" dataDxfId="12" totalsRowDxfId="4"/>
+    <tableColumn id="6" name="Avisos" totalsRowFunction="count" dataDxfId="11" totalsRowDxfId="5"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium25" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="TbLancamentos" displayName="TbLancamentos" ref="A3:E8" totalsRowCount="1" headerRowDxfId="2">
-  <autoFilter ref="A3:E7"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="TbLancamentos" displayName="TbLancamentos" ref="A3:E6" headerRowDxfId="10">
+  <autoFilter ref="A3:E6"/>
   <tableColumns count="5">
     <tableColumn id="1" name="Produto" totalsRowLabel="Total"/>
-    <tableColumn id="2" name="Data" totalsRowFunction="count" dataDxfId="12" totalsRowDxfId="3"/>
-    <tableColumn id="3" name="Entrada" totalsRowFunction="sum" dataDxfId="11"/>
-    <tableColumn id="4" name="Saída" totalsRowFunction="sum" dataDxfId="10"/>
-    <tableColumn id="5" name="Saldo" totalsRowFunction="count" dataDxfId="9" totalsRowDxfId="4"/>
+    <tableColumn id="2" name="Data" totalsRowFunction="count" dataDxfId="9" totalsRowDxfId="0"/>
+    <tableColumn id="3" name="Entrada" totalsRowFunction="sum" dataDxfId="8" totalsRowDxfId="1"/>
+    <tableColumn id="4" name="Saída" totalsRowFunction="sum" dataDxfId="7" totalsRowDxfId="2"/>
+    <tableColumn id="5" name="Saldo" totalsRowFunction="count" dataDxfId="6" totalsRowDxfId="3"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium25" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -2295,10 +2302,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G8"/>
+  <dimension ref="A1:G6"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="G3" sqref="G3"/>
+      <selection activeCell="A4" sqref="A4:A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="0" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2321,22 +2328,22 @@
       <c r="G1" s="1"/>
     </row>
     <row r="3" spans="1:7" s="3" customFormat="1" ht="34.5" x14ac:dyDescent="0.25">
-      <c r="A3" s="14" t="s">
+      <c r="A3" s="13" t="s">
         <v>3</v>
       </c>
-      <c r="B3" s="9" t="s">
+      <c r="B3" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="C3" s="10" t="s">
+      <c r="C3" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="D3" s="10" t="s">
+      <c r="D3" s="9" t="s">
         <v>6</v>
       </c>
-      <c r="E3" s="11" t="s">
+      <c r="E3" s="10" t="s">
         <v>7</v>
       </c>
-      <c r="F3" s="11" t="s">
+      <c r="F3" s="10" t="s">
         <v>8</v>
       </c>
     </row>
@@ -2347,10 +2354,10 @@
       <c r="B4" t="s">
         <v>11</v>
       </c>
-      <c r="C4" s="12">
+      <c r="C4" s="11">
         <v>15</v>
       </c>
-      <c r="D4" s="12">
+      <c r="D4" s="11">
         <v>150</v>
       </c>
       <c r="E4" s="5"/>
@@ -2363,36 +2370,30 @@
       <c r="B5" t="s">
         <v>11</v>
       </c>
-      <c r="C5" s="12">
+      <c r="C5" s="11">
         <v>15</v>
       </c>
-      <c r="D5" s="12">
+      <c r="D5" s="11">
         <v>150</v>
       </c>
       <c r="E5" s="5"/>
       <c r="F5" s="5"/>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="C6" s="12"/>
-      <c r="D6" s="12"/>
+      <c r="A6" t="s">
+        <v>15</v>
+      </c>
+      <c r="B6" t="s">
+        <v>11</v>
+      </c>
+      <c r="C6" s="11">
+        <v>15</v>
+      </c>
+      <c r="D6" s="11">
+        <v>150</v>
+      </c>
       <c r="E6" s="5"/>
       <c r="F6" s="5"/>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="C7" s="12"/>
-      <c r="D7" s="12"/>
-      <c r="E7" s="5"/>
-      <c r="F7" s="5"/>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>15</v>
-      </c>
-      <c r="E8" s="5"/>
-      <c r="F8" s="5">
-        <f>SUBTOTAL(103,TbCadastro[Avisos])</f>
-        <v>0</v>
-      </c>
     </row>
   </sheetData>
   <hyperlinks>
@@ -2409,10 +2410,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G8"/>
+  <dimension ref="A1:G6"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="A7" sqref="A7:XFD7"/>
+      <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="0" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2435,19 +2436,19 @@
       <c r="G1" s="1"/>
     </row>
     <row r="3" spans="1:7" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="16" t="s">
+      <c r="A3" s="14" t="s">
         <v>3</v>
       </c>
-      <c r="B3" s="17" t="s">
+      <c r="B3" s="15" t="s">
         <v>12</v>
       </c>
-      <c r="C3" s="18" t="s">
+      <c r="C3" s="16" t="s">
         <v>14</v>
       </c>
-      <c r="D3" s="19" t="s">
+      <c r="D3" s="17" t="s">
         <v>13</v>
       </c>
-      <c r="E3" s="16" t="s">
+      <c r="E3" s="14" t="s">
         <v>7</v>
       </c>
     </row>
@@ -2455,66 +2456,53 @@
       <c r="A4" t="s">
         <v>9</v>
       </c>
-      <c r="B4" s="7">
+      <c r="B4" s="6">
         <v>44978</v>
       </c>
-      <c r="C4" s="12">
+      <c r="C4" s="11">
         <v>20</v>
       </c>
-      <c r="D4" s="12">
+      <c r="D4" s="11">
         <v>10</v>
       </c>
-      <c r="E4" s="13"/>
+      <c r="E4" s="12"/>
     </row>
     <row r="5" spans="1:7" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
+        <v>9</v>
+      </c>
+      <c r="B5" s="7">
+        <v>44979</v>
+      </c>
+      <c r="C5" s="11">
         <v>10</v>
       </c>
-      <c r="B5" s="8">
-        <v>44979</v>
-      </c>
-      <c r="C5" s="12">
-        <v>10</v>
-      </c>
-      <c r="D5" s="12">
+      <c r="D5" s="11">
         <v>5</v>
       </c>
-      <c r="E5" s="13"/>
+      <c r="E5" s="12"/>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B6" s="8"/>
-      <c r="C6" s="12"/>
-      <c r="D6" s="12"/>
-      <c r="E6" s="13"/>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B7" s="6"/>
-      <c r="C7" s="12"/>
-      <c r="D7" s="12"/>
-      <c r="E7" s="4"/>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
+      <c r="A6" t="s">
         <v>15</v>
       </c>
-      <c r="B8" s="15">
-        <f>SUBTOTAL(103,TbLancamentos[Data])</f>
-        <v>2</v>
-      </c>
-      <c r="C8" s="12">
-        <f>SUBTOTAL(109,TbLancamentos[Entrada])</f>
-        <v>30</v>
-      </c>
-      <c r="D8" s="12">
-        <f>SUBTOTAL(109,TbLancamentos[Saída])</f>
-        <v>15</v>
-      </c>
-      <c r="E8" s="4">
-        <f>SUBTOTAL(103,TbLancamentos[Saldo])</f>
-        <v>0</v>
-      </c>
+      <c r="B6" s="7">
+        <v>44980</v>
+      </c>
+      <c r="C6" s="11">
+        <v>10</v>
+      </c>
+      <c r="D6" s="11">
+        <v>6</v>
+      </c>
+      <c r="E6" s="4"/>
     </row>
   </sheetData>
+  <dataValidations count="1">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A4:A6">
+      <formula1>ColunaProdutos</formula1>
+    </dataValidation>
+  </dataValidations>
   <hyperlinks>
     <hyperlink ref="A1" location="Lançamentos!G1" display="Lançamentos!G1"/>
   </hyperlinks>

</xml_diff>

<commit_message>
Módulo 09 - Projeto estoque part 06 - se
</commit_message>
<xml_diff>
--- a/projeto estoque/Projeto estoque.xlsx
+++ b/projeto estoque/Projeto estoque.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="8670" windowHeight="6180" firstSheet="1" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="8670" windowHeight="6180" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Início" sheetId="1" r:id="rId1"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="18">
   <si>
     <t>Início!G1</t>
   </si>
@@ -82,6 +82,9 @@
   </si>
   <si>
     <t>Para selecionar uma coluna na própria tabela basta abrir colvhetes e selecionar a coluna com tab, e para selecionar o valor na mesma linha basta abrir colchetes inserir o @ e selecionar o nome da coluna na tabela</t>
+  </si>
+  <si>
+    <t>Borracha</t>
   </si>
 </sst>
 </file>
@@ -175,7 +178,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1" applyFill="1"/>
@@ -217,6 +220,14 @@
       <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hiperlink" xfId="1" builtinId="8"/>
@@ -228,11 +239,30 @@
       <fill>
         <patternFill patternType="solid">
           <fgColor indexed="64"/>
+          <bgColor theme="0" tint="-0.14999847407452621"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="0" tint="-0.14999847407452621"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
           <bgColor theme="0" tint="-0.249977111117893"/>
         </patternFill>
       </fill>
     </dxf>
     <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
       <fill>
         <patternFill patternType="solid">
           <fgColor indexed="64"/>
@@ -282,23 +312,6 @@
       </fill>
     </dxf>
     <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="0" tint="-0.14999847407452621"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="0" tint="-0.14999847407452621"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
       <fill>
         <patternFill patternType="solid">
           <fgColor indexed="64"/>
@@ -1979,31 +1992,35 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="TbCadastro" displayName="TbCadastro" ref="A3:F6" headerRowDxfId="15">
-  <autoFilter ref="A3:F6"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="TbCadastro" displayName="TbCadastro" ref="A3:F7" headerRowDxfId="15">
+  <autoFilter ref="A3:F7"/>
   <tableColumns count="6">
     <tableColumn id="1" name="Produto" totalsRowLabel="Total"/>
     <tableColumn id="2" name="Medida"/>
     <tableColumn id="3" name="Estoque_x000a_mínimo" dataDxfId="14"/>
     <tableColumn id="4" name="Estoque_x000a_máximo" dataDxfId="13"/>
-    <tableColumn id="5" name="Saldo" dataDxfId="12" totalsRowDxfId="11">
+    <tableColumn id="5" name="Saldo" dataDxfId="1" totalsRowDxfId="12">
       <calculatedColumnFormula>SUMIF(TbLancamentos[Produto],TbCadastro[[#This Row],[Produto]],TbLancamentos[Entrada])-SUMIF(TbLancamentos[Produto],TbCadastro[[#This Row],[Produto]],TbLancamentos[Saída])</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="6" name="Avisos" totalsRowFunction="count" dataDxfId="10" totalsRowDxfId="9"/>
+    <tableColumn id="6" name="Avisos" totalsRowFunction="count" dataDxfId="0" totalsRowDxfId="11">
+      <calculatedColumnFormula>IF(TbCadastro[[#This Row],[Saldo]]&lt; TbCadastro[[#This Row],[Estoque
+mínimo]],"Solicitar nova compra",IF(TbCadastro[[#This Row],[Saldo]]&gt;=TbCadastro[[#This Row],[Estoque
+máximo]],"Priorizar venda",""))</calculatedColumnFormula>
+    </tableColumn>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium25" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="TbLancamentos" displayName="TbLancamentos" ref="A3:E7" headerRowDxfId="8">
-  <autoFilter ref="A3:E7"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="TbLancamentos" displayName="TbLancamentos" ref="A3:E8" headerRowDxfId="10">
+  <autoFilter ref="A3:E8"/>
   <tableColumns count="5">
     <tableColumn id="1" name="Produto" totalsRowLabel="Total"/>
-    <tableColumn id="2" name="Data" totalsRowFunction="count" dataDxfId="7" totalsRowDxfId="6"/>
-    <tableColumn id="3" name="Entrada" totalsRowFunction="sum" dataDxfId="5" totalsRowDxfId="4"/>
-    <tableColumn id="4" name="Saída" totalsRowFunction="sum" dataDxfId="3" totalsRowDxfId="2"/>
-    <tableColumn id="5" name="Saldo" totalsRowFunction="count" dataDxfId="0" totalsRowDxfId="1">
+    <tableColumn id="2" name="Data" totalsRowFunction="count" dataDxfId="9" totalsRowDxfId="8"/>
+    <tableColumn id="3" name="Entrada" totalsRowFunction="sum" dataDxfId="7" totalsRowDxfId="6"/>
+    <tableColumn id="4" name="Saída" totalsRowFunction="sum" dataDxfId="5" totalsRowDxfId="4"/>
+    <tableColumn id="5" name="Saldo" totalsRowFunction="count" dataDxfId="3" totalsRowDxfId="2">
       <calculatedColumnFormula>SUMIFS(TbLancamentos[Entrada],TbLancamentos[Produto],TbLancamentos[[#This Row],[Produto]],TbLancamentos[Data],"&lt;="&amp;TbLancamentos[[#This Row],[Data]])-SUMIFS(TbLancamentos[Saída],TbLancamentos[Produto],TbLancamentos[[#This Row],[Produto]],TbLancamentos[Data],"&lt;="&amp;TbLancamentos[[#This Row],[Data]])</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -2312,16 +2329,17 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G6"/>
+  <dimension ref="A1:G7"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="E4" sqref="E4"/>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+      <selection activeCell="F4" sqref="F4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="0" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="40.7109375" customWidth="1"/>
-    <col min="2" max="6" width="15.7109375" customWidth="1"/>
+    <col min="2" max="5" width="15.7109375" customWidth="1"/>
+    <col min="6" max="6" width="21.7109375" customWidth="1"/>
     <col min="7" max="7" width="68.42578125" customWidth="1"/>
     <col min="8" max="16384" width="9.140625" hidden="1"/>
   </cols>
@@ -2372,9 +2390,14 @@
       </c>
       <c r="E4" s="5">
         <f>SUMIF(TbLancamentos[Produto],TbCadastro[[#This Row],[Produto]],TbLancamentos[Entrada])-SUMIF(TbLancamentos[Produto],TbCadastro[[#This Row],[Produto]],TbLancamentos[Saída])</f>
-        <v>25</v>
-      </c>
-      <c r="F4" s="5"/>
+        <v>23</v>
+      </c>
+      <c r="F4" s="19" t="str">
+        <f>IF(TbCadastro[[#This Row],[Saldo]]&lt; TbCadastro[[#This Row],[Estoque
+mínimo]],"Solicitar nova compra",IF(TbCadastro[[#This Row],[Saldo]]&gt;=TbCadastro[[#This Row],[Estoque
+máximo]],"Priorizar venda",""))</f>
+        <v/>
+      </c>
     </row>
     <row r="5" spans="1:7" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
@@ -2393,7 +2416,12 @@
         <f>SUMIF(TbLancamentos[Produto],TbCadastro[[#This Row],[Produto]],TbLancamentos[Entrada])-SUMIF(TbLancamentos[Produto],TbCadastro[[#This Row],[Produto]],TbLancamentos[Saída])</f>
         <v>5</v>
       </c>
-      <c r="F5" s="5"/>
+      <c r="F5" s="19" t="str">
+        <f>IF(TbCadastro[[#This Row],[Saldo]]&lt; TbCadastro[[#This Row],[Estoque
+mínimo]],"Solicitar nova compra",IF(TbCadastro[[#This Row],[Saldo]]&gt;=TbCadastro[[#This Row],[Estoque
+máximo]],"Priorizar venda",""))</f>
+        <v>Solicitar nova compra</v>
+      </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
@@ -2412,7 +2440,36 @@
         <f>SUMIF(TbLancamentos[Produto],TbCadastro[[#This Row],[Produto]],TbLancamentos[Entrada])-SUMIF(TbLancamentos[Produto],TbCadastro[[#This Row],[Produto]],TbLancamentos[Saída])</f>
         <v>4</v>
       </c>
-      <c r="F6" s="5"/>
+      <c r="F6" s="19" t="str">
+        <f>IF(TbCadastro[[#This Row],[Saldo]]&lt; TbCadastro[[#This Row],[Estoque
+mínimo]],"Solicitar nova compra",IF(TbCadastro[[#This Row],[Saldo]]&gt;=TbCadastro[[#This Row],[Estoque
+máximo]],"Priorizar venda",""))</f>
+        <v>Solicitar nova compra</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>17</v>
+      </c>
+      <c r="B7" t="s">
+        <v>11</v>
+      </c>
+      <c r="C7" s="11">
+        <v>4</v>
+      </c>
+      <c r="D7" s="11">
+        <v>12</v>
+      </c>
+      <c r="E7" s="20">
+        <f>SUMIF(TbLancamentos[Produto],TbCadastro[[#This Row],[Produto]],TbLancamentos[Entrada])-SUMIF(TbLancamentos[Produto],TbCadastro[[#This Row],[Produto]],TbLancamentos[Saída])</f>
+        <v>17</v>
+      </c>
+      <c r="F7" s="21" t="str">
+        <f>IF(TbCadastro[[#This Row],[Saldo]]&lt; TbCadastro[[#This Row],[Estoque
+mínimo]],"Solicitar nova compra",IF(TbCadastro[[#This Row],[Saldo]]&gt;=TbCadastro[[#This Row],[Estoque
+máximo]],"Priorizar venda",""))</f>
+        <v>Priorizar venda</v>
+      </c>
     </row>
   </sheetData>
   <hyperlinks>
@@ -2431,8 +2488,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G10"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="A10" sqref="A10"/>
+    <sheetView showGridLines="0" workbookViewId="0">
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="0" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2499,10 +2556,12 @@
       <c r="C5" s="11">
         <v>10</v>
       </c>
-      <c r="D5" s="11"/>
+      <c r="D5" s="11">
+        <v>2</v>
+      </c>
       <c r="E5" s="18">
         <f>SUMIFS(TbLancamentos[Entrada],TbLancamentos[Produto],TbLancamentos[[#This Row],[Produto]],TbLancamentos[Data],"&lt;="&amp;TbLancamentos[[#This Row],[Data]])-SUMIFS(TbLancamentos[Saída],TbLancamentos[Produto],TbLancamentos[[#This Row],[Produto]],TbLancamentos[Data],"&lt;="&amp;TbLancamentos[[#This Row],[Data]])</f>
-        <v>25</v>
+        <v>23</v>
       </c>
     </row>
     <row r="6" spans="1:7" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -2541,6 +2600,24 @@
         <v>4</v>
       </c>
     </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>17</v>
+      </c>
+      <c r="B8" s="7">
+        <v>44981</v>
+      </c>
+      <c r="C8" s="11">
+        <v>19</v>
+      </c>
+      <c r="D8" s="11">
+        <v>2</v>
+      </c>
+      <c r="E8" s="22">
+        <f>SUMIFS(TbLancamentos[Entrada],TbLancamentos[Produto],TbLancamentos[[#This Row],[Produto]],TbLancamentos[Data],"&lt;="&amp;TbLancamentos[[#This Row],[Data]])-SUMIFS(TbLancamentos[Saída],TbLancamentos[Produto],TbLancamentos[[#This Row],[Produto]],TbLancamentos[Data],"&lt;="&amp;TbLancamentos[[#This Row],[Data]])</f>
+        <v>17</v>
+      </c>
+    </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>16</v>
@@ -2548,7 +2625,7 @@
     </row>
   </sheetData>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A4:A7">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A4:A8">
       <formula1>ColunaProdutos</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>

<commit_message>
Módulo 09 - Projeto estoque part 06 - ajustes
</commit_message>
<xml_diff>
--- a/projeto estoque/Projeto estoque.xlsx
+++ b/projeto estoque/Projeto estoque.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="8670" windowHeight="6180" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="8670" windowHeight="6180" firstSheet="2" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Início" sheetId="1" r:id="rId1"/>
@@ -233,25 +233,63 @@
     <cellStyle name="Hiperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="16">
+  <dxfs count="22">
     <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color theme="0"/>
+      </font>
       <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="0" tint="-0.14999847407452621"/>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
         </patternFill>
       </fill>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color theme="0"/>
+      </font>
       <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="0" tint="-0.14999847407452621"/>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
         </patternFill>
       </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FFC00000"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color theme="5"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FFC00000"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FFC00000"/>
+      </font>
     </dxf>
     <dxf>
       <fill>
@@ -312,6 +350,25 @@
       </fill>
     </dxf>
     <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="0" tint="-0.14999847407452621"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="0" tint="-0.14999847407452621"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
       <fill>
         <patternFill patternType="solid">
           <fgColor indexed="64"/>
@@ -1992,17 +2049,17 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="TbCadastro" displayName="TbCadastro" ref="A3:F7" headerRowDxfId="15">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="TbCadastro" displayName="TbCadastro" ref="A3:F7" headerRowDxfId="21">
   <autoFilter ref="A3:F7"/>
   <tableColumns count="6">
     <tableColumn id="1" name="Produto" totalsRowLabel="Total"/>
     <tableColumn id="2" name="Medida"/>
-    <tableColumn id="3" name="Estoque_x000a_mínimo" dataDxfId="14"/>
-    <tableColumn id="4" name="Estoque_x000a_máximo" dataDxfId="13"/>
-    <tableColumn id="5" name="Saldo" dataDxfId="1" totalsRowDxfId="12">
+    <tableColumn id="3" name="Estoque_x000a_mínimo" dataDxfId="20"/>
+    <tableColumn id="4" name="Estoque_x000a_máximo" dataDxfId="19"/>
+    <tableColumn id="5" name="Saldo" dataDxfId="18" totalsRowDxfId="17">
       <calculatedColumnFormula>SUMIF(TbLancamentos[Produto],TbCadastro[[#This Row],[Produto]],TbLancamentos[Entrada])-SUMIF(TbLancamentos[Produto],TbCadastro[[#This Row],[Produto]],TbLancamentos[Saída])</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="6" name="Avisos" totalsRowFunction="count" dataDxfId="0" totalsRowDxfId="11">
+    <tableColumn id="6" name="Avisos" totalsRowFunction="count" dataDxfId="16" totalsRowDxfId="15">
       <calculatedColumnFormula>IF(TbCadastro[[#This Row],[Saldo]]&lt; TbCadastro[[#This Row],[Estoque
 mínimo]],"Solicitar nova compra",IF(TbCadastro[[#This Row],[Saldo]]&gt;=TbCadastro[[#This Row],[Estoque
 máximo]],"Priorizar venda",""))</calculatedColumnFormula>
@@ -2013,14 +2070,14 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="TbLancamentos" displayName="TbLancamentos" ref="A3:E8" headerRowDxfId="10">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="TbLancamentos" displayName="TbLancamentos" ref="A3:E8" headerRowDxfId="14">
   <autoFilter ref="A3:E8"/>
   <tableColumns count="5">
     <tableColumn id="1" name="Produto" totalsRowLabel="Total"/>
-    <tableColumn id="2" name="Data" totalsRowFunction="count" dataDxfId="9" totalsRowDxfId="8"/>
-    <tableColumn id="3" name="Entrada" totalsRowFunction="sum" dataDxfId="7" totalsRowDxfId="6"/>
-    <tableColumn id="4" name="Saída" totalsRowFunction="sum" dataDxfId="5" totalsRowDxfId="4"/>
-    <tableColumn id="5" name="Saldo" totalsRowFunction="count" dataDxfId="3" totalsRowDxfId="2">
+    <tableColumn id="2" name="Data" totalsRowFunction="count" dataDxfId="13" totalsRowDxfId="12"/>
+    <tableColumn id="3" name="Entrada" totalsRowFunction="sum" dataDxfId="11" totalsRowDxfId="10"/>
+    <tableColumn id="4" name="Saída" totalsRowFunction="sum" dataDxfId="9" totalsRowDxfId="8"/>
+    <tableColumn id="5" name="Saldo" totalsRowFunction="count" dataDxfId="7" totalsRowDxfId="6">
       <calculatedColumnFormula>SUMIFS(TbLancamentos[Entrada],TbLancamentos[Produto],TbLancamentos[[#This Row],[Produto]],TbLancamentos[Data],"&lt;="&amp;TbLancamentos[[#This Row],[Data]])-SUMIFS(TbLancamentos[Saída],TbLancamentos[Produto],TbLancamentos[[#This Row],[Produto]],TbLancamentos[Data],"&lt;="&amp;TbLancamentos[[#This Row],[Data]])</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -2331,8 +2388,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G7"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="F4" sqref="F4"/>
+    <sheetView showGridLines="0" topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="G9" sqref="G9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="0" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2438,7 +2495,7 @@
       </c>
       <c r="E6" s="5">
         <f>SUMIF(TbLancamentos[Produto],TbCadastro[[#This Row],[Produto]],TbLancamentos[Entrada])-SUMIF(TbLancamentos[Produto],TbCadastro[[#This Row],[Produto]],TbLancamentos[Saída])</f>
-        <v>4</v>
+        <v>-3</v>
       </c>
       <c r="F6" s="19" t="str">
         <f>IF(TbCadastro[[#This Row],[Saldo]]&lt; TbCadastro[[#This Row],[Estoque
@@ -2472,6 +2529,14 @@
       </c>
     </row>
   </sheetData>
+  <conditionalFormatting sqref="F4:F7">
+    <cfRule type="cellIs" dxfId="4" priority="2" operator="equal">
+      <formula>"Solicitar nova compra"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="3" priority="1" operator="equal">
+      <formula>"Priorizar venda"</formula>
+    </cfRule>
+  </conditionalFormatting>
   <hyperlinks>
     <hyperlink ref="A1" location="Cadastro!G1" display="Cadastro!G1"/>
   </hyperlinks>
@@ -2488,8 +2553,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G10"/>
   <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="0" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2593,11 +2658,11 @@
         <v>10</v>
       </c>
       <c r="D7" s="11">
-        <v>6</v>
+        <v>13</v>
       </c>
       <c r="E7" s="4">
         <f>SUMIFS(TbLancamentos[Entrada],TbLancamentos[Produto],TbLancamentos[[#This Row],[Produto]],TbLancamentos[Data],"&lt;="&amp;TbLancamentos[[#This Row],[Data]])-SUMIFS(TbLancamentos[Saída],TbLancamentos[Produto],TbLancamentos[[#This Row],[Produto]],TbLancamentos[Data],"&lt;="&amp;TbLancamentos[[#This Row],[Data]])</f>
-        <v>4</v>
+        <v>-3</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
@@ -2624,6 +2689,11 @@
       </c>
     </row>
   </sheetData>
+  <conditionalFormatting sqref="E4:E8">
+    <cfRule type="cellIs" dxfId="1" priority="1" operator="lessThan">
+      <formula>0</formula>
+    </cfRule>
+  </conditionalFormatting>
   <dataValidations count="1">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A4:A8">
       <formula1>ColunaProdutos</formula1>

</xml_diff>

<commit_message>
Módulo 09 - Projeto estoque - finalização
</commit_message>
<xml_diff>
--- a/projeto estoque/Projeto estoque.xlsx
+++ b/projeto estoque/Projeto estoque.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="8670" windowHeight="6180" firstSheet="2" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="8670" windowHeight="6180" firstSheet="1" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Início" sheetId="1" r:id="rId1"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="21">
   <si>
     <t>Início!G1</t>
   </si>
@@ -85,6 +85,15 @@
   </si>
   <si>
     <t>Borracha</t>
+  </si>
+  <si>
+    <t>Impedir que o gráfico mude de tamanho</t>
+  </si>
+  <si>
+    <t>Clica no gráfico/formatar/tamanho/menu propriedades</t>
+  </si>
+  <si>
+    <t>marca a opção : não mover ou dimnensionar com células</t>
   </si>
 </sst>
 </file>
@@ -233,64 +242,7 @@
     <cellStyle name="Hiperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="22">
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FFC00000"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color theme="5"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FFC00000"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FFC00000"/>
-      </font>
-    </dxf>
+  <dxfs count="19">
     <dxf>
       <fill>
         <patternFill patternType="solid">
@@ -340,6 +292,18 @@
         <scheme val="minor"/>
       </font>
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
     </dxf>
     <dxf>
       <fill>
@@ -396,6 +360,25 @@
       </font>
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color theme="5"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FFC00000"/>
+      </font>
+    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
@@ -407,6 +390,801 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="pt-BR"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:autoTitleDeleted val="1"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:doughnutChart>
+        <c:varyColors val="1"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Cadastro!$E$3</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Saldo</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:dPt>
+            <c:idx val="0"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="19050">
+                <a:solidFill>
+                  <a:schemeClr val="lt1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="1"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:ln w="19050">
+                <a:solidFill>
+                  <a:schemeClr val="lt1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="2"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent3"/>
+              </a:solidFill>
+              <a:ln w="19050">
+                <a:solidFill>
+                  <a:schemeClr val="lt1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="3"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent4"/>
+              </a:solidFill>
+              <a:ln w="19050">
+                <a:solidFill>
+                  <a:schemeClr val="lt1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:dPt>
+          <c:dLbls>
+            <c:numFmt formatCode="0%" sourceLinked="0"/>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1100" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="75000"/>
+                        <a:lumOff val="25000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="pt-BR"/>
+              </a:p>
+            </c:txPr>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="0"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="1"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:layout/>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
+          <c:cat>
+            <c:strRef>
+              <c:f>Cadastro!$A$4:$A$7</c:f>
+              <c:strCache>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>Caneta esferográfica azul</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Caneta esferográfica preta</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Lápis</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Borracha</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Cadastro!$E$4:$E$7</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>23</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>-3</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>17</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="1"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+          <c:showLeaderLines val="0"/>
+        </c:dLbls>
+        <c:firstSliceAng val="0"/>
+        <c:holeSize val="63"/>
+      </c:doughnutChart>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="pt-BR"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.78740157499999996" l="0.511811024" r="0.511811024" t="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="251">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050">
+        <a:solidFill>
+          <a:schemeClr val="lt1"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="25400">
+        <a:solidFill>
+          <a:schemeClr val="lt1"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
 </file>
 
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1550,6 +2328,100 @@
     </xdr:sp>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="absolute">
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>76200</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>228599</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>4171950</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>28575</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="7" name="Gráfico 6"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId4"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>642938</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>76201</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>4214813</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>228601</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="8" name="CaixaDeTexto 7"/>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="8996363" y="704851"/>
+          <a:ext cx="3571875" cy="342900"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="lt1"/>
+        </a:solidFill>
+        <a:ln w="9525" cmpd="sng">
+          <a:noFill/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr lang="pt-BR" sz="1400" b="1">
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+            </a:rPr>
+            <a:t>Composição do saldo atual do estoque</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
 
@@ -2049,17 +2921,17 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="TbCadastro" displayName="TbCadastro" ref="A3:F7" headerRowDxfId="21">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="TbCadastro" displayName="TbCadastro" ref="A3:F7" headerRowDxfId="16">
   <autoFilter ref="A3:F7"/>
   <tableColumns count="6">
     <tableColumn id="1" name="Produto" totalsRowLabel="Total"/>
     <tableColumn id="2" name="Medida"/>
-    <tableColumn id="3" name="Estoque_x000a_mínimo" dataDxfId="20"/>
-    <tableColumn id="4" name="Estoque_x000a_máximo" dataDxfId="19"/>
-    <tableColumn id="5" name="Saldo" dataDxfId="18" totalsRowDxfId="17">
+    <tableColumn id="3" name="Estoque_x000a_mínimo" dataDxfId="15"/>
+    <tableColumn id="4" name="Estoque_x000a_máximo" dataDxfId="14"/>
+    <tableColumn id="5" name="Saldo" dataDxfId="13" totalsRowDxfId="12">
       <calculatedColumnFormula>SUMIF(TbLancamentos[Produto],TbCadastro[[#This Row],[Produto]],TbLancamentos[Entrada])-SUMIF(TbLancamentos[Produto],TbCadastro[[#This Row],[Produto]],TbLancamentos[Saída])</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="6" name="Avisos" totalsRowFunction="count" dataDxfId="16" totalsRowDxfId="15">
+    <tableColumn id="6" name="Avisos" totalsRowFunction="count" dataDxfId="11" totalsRowDxfId="10">
       <calculatedColumnFormula>IF(TbCadastro[[#This Row],[Saldo]]&lt; TbCadastro[[#This Row],[Estoque
 mínimo]],"Solicitar nova compra",IF(TbCadastro[[#This Row],[Saldo]]&gt;=TbCadastro[[#This Row],[Estoque
 máximo]],"Priorizar venda",""))</calculatedColumnFormula>
@@ -2070,14 +2942,14 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="TbLancamentos" displayName="TbLancamentos" ref="A3:E8" headerRowDxfId="14">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="TbLancamentos" displayName="TbLancamentos" ref="A3:E8" headerRowDxfId="8">
   <autoFilter ref="A3:E8"/>
   <tableColumns count="5">
     <tableColumn id="1" name="Produto" totalsRowLabel="Total"/>
-    <tableColumn id="2" name="Data" totalsRowFunction="count" dataDxfId="13" totalsRowDxfId="12"/>
-    <tableColumn id="3" name="Entrada" totalsRowFunction="sum" dataDxfId="11" totalsRowDxfId="10"/>
-    <tableColumn id="4" name="Saída" totalsRowFunction="sum" dataDxfId="9" totalsRowDxfId="8"/>
-    <tableColumn id="5" name="Saldo" totalsRowFunction="count" dataDxfId="7" totalsRowDxfId="6">
+    <tableColumn id="2" name="Data" totalsRowFunction="count" dataDxfId="7" totalsRowDxfId="6"/>
+    <tableColumn id="3" name="Entrada" totalsRowFunction="sum" dataDxfId="5" totalsRowDxfId="4"/>
+    <tableColumn id="4" name="Saída" totalsRowFunction="sum" dataDxfId="3" totalsRowDxfId="2"/>
+    <tableColumn id="5" name="Saldo" totalsRowFunction="count" dataDxfId="1" totalsRowDxfId="0">
       <calculatedColumnFormula>SUMIFS(TbLancamentos[Entrada],TbLancamentos[Produto],TbLancamentos[[#This Row],[Produto]],TbLancamentos[Data],"&lt;="&amp;TbLancamentos[[#This Row],[Data]])-SUMIFS(TbLancamentos[Saída],TbLancamentos[Produto],TbLancamentos[[#This Row],[Produto]],TbLancamentos[Data],"&lt;="&amp;TbLancamentos[[#This Row],[Data]])</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -2386,10 +3258,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G7"/>
+  <dimension ref="A1:G14"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="G9" sqref="G9"/>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="0" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2528,12 +3400,27 @@
         <v>Priorizar venda</v>
       </c>
     </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>20</v>
+      </c>
+    </row>
   </sheetData>
   <conditionalFormatting sqref="F4:F7">
-    <cfRule type="cellIs" dxfId="4" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="18" priority="2" operator="equal">
       <formula>"Solicitar nova compra"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="3" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="17" priority="1" operator="equal">
       <formula>"Priorizar venda"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -2553,8 +3440,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G10"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+    <sheetView showGridLines="0" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="0" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2690,7 +3577,7 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="E4:E8">
-    <cfRule type="cellIs" dxfId="1" priority="1" operator="lessThan">
+    <cfRule type="cellIs" dxfId="9" priority="1" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
Módulo 09 - Projeto estoque - finalização 2
</commit_message>
<xml_diff>
--- a/projeto estoque/Projeto estoque.xlsx
+++ b/projeto estoque/Projeto estoque.xlsx
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="22">
   <si>
     <t>Início!G1</t>
   </si>
@@ -94,6 +94,9 @@
   </si>
   <si>
     <t>marca a opção : não mover ou dimnensionar com células</t>
+  </si>
+  <si>
+    <t>Outra aba importante: clica no gráfico/formatar/formatar seleção</t>
   </si>
 </sst>
 </file>
@@ -3258,10 +3261,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G14"/>
+  <dimension ref="A1:G15"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+      <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="0" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3413,6 +3416,11 @@
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>20</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>21</v>
       </c>
     </row>
   </sheetData>

</xml_diff>